<commit_message>
Added colour coding to themes
</commit_message>
<xml_diff>
--- a/Design debt.xlsx
+++ b/Design debt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="17060" yWindow="0" windowWidth="34120" windowHeight="27260" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="3" r:id="rId1"/>
@@ -643,7 +643,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -707,19 +707,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="24"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -729,19 +716,47 @@
       <sz val="12"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFFFC000"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -777,6 +792,54 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF009950"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD53880"/>
+        <bgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF28A197"/>
+        <bgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF47738"/>
+        <bgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF005EA5"/>
+        <bgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF912B88"/>
+        <bgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDF3034"/>
+        <bgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2E358B"/>
+        <bgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF006435"/>
+        <bgColor rgb="FFFFC000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1045,7 +1108,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1053,7 +1116,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1066,7 +1129,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1075,29 +1138,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1106,22 +1151,149 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="14" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="15" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="15" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="15" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="15" fillId="14" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="15" fillId="15" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1722,7 +1894,7 @@
   <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1733,234 +1905,234 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="28">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="12" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="55" customHeight="1">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="2:7" s="17" customFormat="1" ht="43" customHeight="1">
-      <c r="B6" s="20" t="str">
+    <row r="6" spans="2:7" s="11" customFormat="1" ht="43" customHeight="1">
+      <c r="B6" s="14" t="str">
         <f>Heuristics!B2</f>
         <v xml:space="preserve">SEARCH &amp; FINDABILITY </v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="15">
         <f>COUNTA(SEARCH_SCORE)</f>
         <v>11</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="17">
         <f>(COUNTIF(SEARCH_SCORE,0))/(COUNTA(SEARCH_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="18">
         <f>(COUNTIF(SEARCH_SCORE,1))/(COUNTA(SEARCH_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="19">
         <f>(COUNTIF(SEARCH_SCORE,2))/(COUNTA(SEARCH_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="20">
         <f>(COUNTIF(SEARCH_SCORE,3))/(COUNTA(SEARCH_SCORE))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:7" s="17" customFormat="1" ht="43" customHeight="1">
-      <c r="B7" s="20" t="str">
+    <row r="7" spans="2:7" s="11" customFormat="1" ht="43" customHeight="1">
+      <c r="B7" s="14" t="str">
         <f>Heuristics!B17</f>
         <v xml:space="preserve">CLARITY  </v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="15">
         <f>COUNTA(CLARITY_SCORE)</f>
         <v>17</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="17">
         <f>(COUNTIF(CLARITY_SCORE,0))/(COUNTA(CLARITY_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="18">
         <f>(COUNTIF(CLARITY_SCORE,1))/(COUNTA(CLARITY_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="19">
         <f>(COUNTIF(CLARITY_SCORE,2))/(COUNTA(CLARITY_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="20">
         <f>(COUNTIF(CLARITY_SCORE,3))/(COUNTA(CLARITY_SCORE))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:7" s="17" customFormat="1" ht="43" customHeight="1">
-      <c r="B8" s="20" t="str">
+    <row r="8" spans="2:7" s="11" customFormat="1" ht="43" customHeight="1">
+      <c r="B8" s="14" t="str">
         <f>Heuristics!B38</f>
         <v>TRUST &amp; CREDIBILITY</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="15">
         <f>COUNTA(TRUST_SCORE)</f>
         <v>6</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="17">
         <f>(COUNTIF(TRUST_SCORE,0))/(COUNTA(TRUST_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="18">
         <f>(COUNTIF(TRUST_SCORE,1))/(COUNTA(TRUST_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="19">
         <f>(COUNTIF(TRUST_SCORE,2))/(COUNTA(TRUST_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="20">
         <f>(COUNTIF(TRUST_SCORE,3))/(COUNTA(TRUST_SCORE))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:7" s="17" customFormat="1" ht="43" customHeight="1">
-      <c r="B9" s="20" t="str">
+    <row r="9" spans="2:7" s="11" customFormat="1" ht="43" customHeight="1">
+      <c r="B9" s="14" t="str">
         <f>Heuristics!B48</f>
         <v>HELP, FEEDBACK &amp; ERROR TOLLERANCE</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="15">
         <f>COUNTA(HELP_SCORE)</f>
         <v>18</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="17">
         <f>(COUNTIF(HELP_SCORE,0))/(COUNTA(HELP_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="18">
         <f>(COUNTIF(HELP_SCORE,1))/(COUNTA(HELP_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="19">
         <f>(COUNTIF(HELP_SCORE,2))/(COUNTA(HELP_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="20">
         <f>(COUNTIF(HELP_SCORE,3))/(COUNTA(HELP_SCORE))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:7" s="17" customFormat="1" ht="43" customHeight="1">
-      <c r="B10" s="20" t="str">
+    <row r="10" spans="2:7" s="11" customFormat="1" ht="43" customHeight="1">
+      <c r="B10" s="14" t="str">
         <f>Heuristics!B70</f>
         <v>FORMS &amp; DATA ENTRY</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="15">
         <f>COUNTA(FORMS_SCORE)</f>
         <v>15</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="17">
         <f>(COUNTIF(FORMS_SCORE,0))/(COUNTA(FORMS_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="18">
         <f>(COUNTIF(FORMS_SCORE,1))/(COUNTA(FORMS_SCORE))</f>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="19">
         <f>(COUNTIF(FORMS_SCORE,2))/(COUNTA(FORMS_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="20">
         <f>(COUNTIF(FORMS_SCORE,3))/(COUNTA(FORMS_SCORE))</f>
         <v>0.93333333333333335</v>
       </c>
     </row>
-    <row r="11" spans="2:7" s="17" customFormat="1" ht="43" customHeight="1">
-      <c r="B11" s="20" t="str">
+    <row r="11" spans="2:7" s="11" customFormat="1" ht="43" customHeight="1">
+      <c r="B11" s="14" t="str">
         <f>Heuristics!B89</f>
         <v>PERSUASIVE DESIGN</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="15">
         <f>COUNTA(PERSUASIVE_SCORE)</f>
         <v>13</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="17">
         <f>(COUNTIF(PERSUASIVE_SCORE,0))/(COUNTA(PERSUASIVE_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="18">
         <f>(COUNTIF(PERSUASIVE_SCORE,1))/(COUNTA(PERSUASIVE_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="19">
         <f>(COUNTIF(PERSUASIVE_SCORE,2))/(COUNTA(PERSUASIVE_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="20">
         <f>(COUNTIF(PERSUASIVE_SCORE,3))/(COUNTA(PERSUASIVE_SCORE))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:7" s="17" customFormat="1" ht="43" customHeight="1">
-      <c r="B12" s="20" t="str">
+    <row r="12" spans="2:7" s="11" customFormat="1" ht="43" customHeight="1">
+      <c r="B12" s="14" t="str">
         <f>Heuristics!B106</f>
         <v>ACCESSIBILITY</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="15">
         <f>COUNTA(ACCESSIBILITY_SCORE)</f>
         <v>36</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="17">
         <f>(COUNTIF(ACCESSIBILITY_SCORE,0))/(COUNTA(ACCESSIBILITY_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="18">
         <f>(COUNTIF(ACCESSIBILITY_SCORE,1))/(COUNTA(ACCESSIBILITY_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="19">
         <f>(COUNTIF(ACCESSIBILITY_SCORE,2))/(COUNTA(ACCESSIBILITY_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="G12" s="26">
+      <c r="G12" s="20">
         <f>(COUNTIF(ACCESSIBILITY_SCORE,3))/(COUNTA(ACCESSIBILITY_SCORE))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:7" s="17" customFormat="1" ht="43" customHeight="1">
-      <c r="B13" s="20" t="str">
+    <row r="13" spans="2:7" s="11" customFormat="1" ht="43" customHeight="1">
+      <c r="B13" s="14" t="str">
         <f>Heuristics!B146</f>
         <v>TASK FOCUS</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="15">
         <f>COUNTA(SERVICE_SCORE)</f>
         <v>9</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="17">
         <f>(COUNTIF(SERVICE_SCORE,0))/(COUNTA(SERVICE_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="18">
         <f>(COUNTIF(SERVICE_SCORE,1))/(COUNTA(SERVICE_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="19">
         <f>(COUNTIF(SERVICE_SCORE,2))/(COUNTA(SERVICE_SCORE))</f>
         <v>0</v>
       </c>
-      <c r="G13" s="26">
+      <c r="G13" s="20">
         <f>(COUNTIF(SERVICE_SCORE,3))/(COUNTA(SERVICE_SCORE))</f>
         <v>1</v>
       </c>
@@ -1983,8 +2155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFB157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="B168" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2001,31 +2173,29 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="10"/>
-      <c r="C1" s="5"/>
       <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" ht="20">
-      <c r="A2" s="13"/>
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="1:5" s="26" customFormat="1" ht="20">
+      <c r="A2" s="24"/>
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="27" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="13"/>
-      <c r="B3" s="11" t="s">
+    <row r="3" spans="1:5" s="26" customFormat="1" ht="30">
+      <c r="A3" s="24"/>
+      <c r="B3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="6">
@@ -2193,31 +2363,31 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="20">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="23"/>
     </row>
     <row r="17" spans="1:16382" ht="20">
-      <c r="A17" s="13"/>
-      <c r="B17" s="15" t="s">
+      <c r="A17" s="30"/>
+      <c r="B17" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13" t="s">
+      <c r="C17" s="32"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="32" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:16382" ht="45">
-      <c r="A18" s="13"/>
-      <c r="B18" s="11" t="s">
+      <c r="A18" s="30"/>
+      <c r="B18" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="32"/>
     </row>
     <row r="19" spans="1:16382">
       <c r="A19" s="6">
@@ -2323,7 +2493,7 @@
         <f>VLOOKUP(C25,'lookup values'!A$1:B$5,2,0)</f>
         <v>3</v>
       </c>
-      <c r="E25"/>
+      <c r="E25" s="41"/>
       <c r="F25"/>
       <c r="G25"/>
       <c r="H25"/>
@@ -18853,34 +19023,34 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="20">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
+      <c r="A36" s="28"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="29"/>
     </row>
     <row r="37" spans="1:5">
       <c r="C37" s="9"/>
     </row>
     <row r="38" spans="1:5" ht="20">
-      <c r="A38" s="13"/>
-      <c r="B38" s="15" t="s">
+      <c r="A38" s="38"/>
+      <c r="B38" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13" t="s">
+      <c r="C38" s="40"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="40" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="45">
-      <c r="A39" s="13"/>
-      <c r="B39" s="11" t="s">
+      <c r="A39" s="38"/>
+      <c r="B39" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="40"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="6">
@@ -18973,34 +19143,34 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="20">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
+      <c r="A46" s="33"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="34"/>
     </row>
     <row r="47" spans="1:5">
       <c r="C47" s="9"/>
     </row>
     <row r="48" spans="1:5" ht="20">
-      <c r="A48" s="13"/>
-      <c r="B48" s="15" t="s">
+      <c r="A48" s="35"/>
+      <c r="B48" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13" t="s">
+      <c r="C48" s="37"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="37" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="13"/>
-      <c r="B49" s="11" t="s">
+      <c r="A49" s="35"/>
+      <c r="B49" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="37"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="6">
@@ -19273,34 +19443,34 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="20">
-      <c r="A68" s="13"/>
-      <c r="B68" s="13"/>
-      <c r="C68" s="16"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="13"/>
+      <c r="A68" s="35"/>
+      <c r="B68" s="35"/>
+      <c r="C68" s="45"/>
+      <c r="D68" s="35"/>
+      <c r="E68" s="37"/>
     </row>
     <row r="69" spans="1:5">
       <c r="C69" s="9"/>
     </row>
     <row r="70" spans="1:5" ht="20">
-      <c r="A70" s="14"/>
-      <c r="B70" s="15" t="s">
+      <c r="A70" s="46"/>
+      <c r="B70" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="C70" s="13"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="13" t="s">
+      <c r="C70" s="48"/>
+      <c r="D70" s="49"/>
+      <c r="E70" s="48" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="14"/>
-      <c r="B71" s="12" t="s">
+      <c r="A71" s="46"/>
+      <c r="B71" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="C71" s="13"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="13"/>
+      <c r="C71" s="48"/>
+      <c r="D71" s="49"/>
+      <c r="E71" s="48"/>
     </row>
     <row r="72" spans="1:5" ht="30">
       <c r="A72" s="6">
@@ -19528,34 +19698,34 @@
       </c>
     </row>
     <row r="87" spans="1:5" ht="20">
-      <c r="A87" s="13"/>
-      <c r="B87" s="13"/>
-      <c r="C87" s="16"/>
-      <c r="D87" s="13"/>
-      <c r="E87" s="13"/>
+      <c r="A87" s="49"/>
+      <c r="B87" s="49"/>
+      <c r="C87" s="50"/>
+      <c r="D87" s="49"/>
+      <c r="E87" s="48"/>
     </row>
     <row r="88" spans="1:5">
       <c r="C88" s="9"/>
     </row>
     <row r="89" spans="1:5" ht="20">
-      <c r="A89" s="13"/>
-      <c r="B89" s="15" t="s">
+      <c r="A89" s="51"/>
+      <c r="B89" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="C89" s="13"/>
-      <c r="D89" s="13"/>
-      <c r="E89" s="13" t="s">
+      <c r="C89" s="53"/>
+      <c r="D89" s="51"/>
+      <c r="E89" s="53" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="90" spans="1:5">
-      <c r="A90" s="13"/>
-      <c r="B90" s="12" t="s">
+      <c r="A90" s="51"/>
+      <c r="B90" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="C90" s="13"/>
-      <c r="D90" s="13"/>
-      <c r="E90" s="13"/>
+      <c r="C90" s="53"/>
+      <c r="D90" s="51"/>
+      <c r="E90" s="53"/>
     </row>
     <row r="91" spans="1:5" ht="30">
       <c r="A91" s="6">
@@ -19753,37 +19923,37 @@
       </c>
     </row>
     <row r="104" spans="1:5" ht="20">
-      <c r="A104" s="13"/>
-      <c r="B104" s="13"/>
-      <c r="C104" s="16"/>
-      <c r="D104" s="13"/>
-      <c r="E104" s="13"/>
+      <c r="A104" s="51"/>
+      <c r="B104" s="51"/>
+      <c r="C104" s="54"/>
+      <c r="D104" s="51"/>
+      <c r="E104" s="53"/>
     </row>
     <row r="105" spans="1:5">
       <c r="C105" s="9"/>
     </row>
     <row r="106" spans="1:5" ht="23" customHeight="1">
-      <c r="A106" s="13"/>
-      <c r="B106" s="15" t="s">
+      <c r="A106" s="55"/>
+      <c r="B106" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="C106" s="13"/>
-      <c r="D106" s="13"/>
-      <c r="E106" s="13" t="s">
+      <c r="C106" s="57"/>
+      <c r="D106" s="55"/>
+      <c r="E106" s="57" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="30">
-      <c r="A107" s="13"/>
-      <c r="B107" s="11" t="s">
+      <c r="A107" s="55"/>
+      <c r="B107" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="C107" s="13"/>
-      <c r="D107" s="13"/>
-      <c r="E107" s="13"/>
+      <c r="C107" s="57"/>
+      <c r="D107" s="55"/>
+      <c r="E107" s="57"/>
     </row>
     <row r="108" spans="1:5" ht="30">
-      <c r="A108" s="27" t="s">
+      <c r="A108" s="21" t="s">
         <v>111</v>
       </c>
       <c r="B108" s="7" t="s">
@@ -19798,7 +19968,7 @@
       </c>
     </row>
     <row r="109" spans="1:5" ht="30">
-      <c r="A109" s="27" t="s">
+      <c r="A109" s="21" t="s">
         <v>112</v>
       </c>
       <c r="B109" s="7" t="s">
@@ -19813,7 +19983,7 @@
       </c>
     </row>
     <row r="110" spans="1:5" ht="30">
-      <c r="A110" s="27" t="s">
+      <c r="A110" s="21" t="s">
         <v>113</v>
       </c>
       <c r="B110" s="7" t="s">
@@ -19828,7 +19998,7 @@
       </c>
     </row>
     <row r="111" spans="1:5" ht="30">
-      <c r="A111" s="27" t="s">
+      <c r="A111" s="21" t="s">
         <v>114</v>
       </c>
       <c r="B111" s="7" t="s">
@@ -19843,7 +20013,7 @@
       </c>
     </row>
     <row r="112" spans="1:5" ht="30">
-      <c r="A112" s="27" t="s">
+      <c r="A112" s="21" t="s">
         <v>115</v>
       </c>
       <c r="B112" s="7" t="s">
@@ -19858,7 +20028,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="30">
-      <c r="A113" s="27" t="s">
+      <c r="A113" s="21" t="s">
         <v>116</v>
       </c>
       <c r="B113" s="7" t="s">
@@ -19873,7 +20043,7 @@
       </c>
     </row>
     <row r="114" spans="1:4" ht="30">
-      <c r="A114" s="27" t="s">
+      <c r="A114" s="21" t="s">
         <v>117</v>
       </c>
       <c r="B114" s="7" t="s">
@@ -19888,7 +20058,7 @@
       </c>
     </row>
     <row r="115" spans="1:4" ht="30">
-      <c r="A115" s="27" t="s">
+      <c r="A115" s="21" t="s">
         <v>118</v>
       </c>
       <c r="B115" s="7" t="s">
@@ -19903,7 +20073,7 @@
       </c>
     </row>
     <row r="116" spans="1:4" ht="30">
-      <c r="A116" s="27" t="s">
+      <c r="A116" s="21" t="s">
         <v>119</v>
       </c>
       <c r="B116" s="7" t="s">
@@ -19918,7 +20088,7 @@
       </c>
     </row>
     <row r="117" spans="1:4" ht="30">
-      <c r="A117" s="27" t="s">
+      <c r="A117" s="21" t="s">
         <v>120</v>
       </c>
       <c r="B117" s="7" t="s">
@@ -19933,7 +20103,7 @@
       </c>
     </row>
     <row r="118" spans="1:4" ht="30">
-      <c r="A118" s="27" t="s">
+      <c r="A118" s="21" t="s">
         <v>121</v>
       </c>
       <c r="B118" s="7" t="s">
@@ -19948,7 +20118,7 @@
       </c>
     </row>
     <row r="119" spans="1:4" ht="30">
-      <c r="A119" s="27" t="s">
+      <c r="A119" s="21" t="s">
         <v>122</v>
       </c>
       <c r="B119" s="7" t="s">
@@ -19963,7 +20133,7 @@
       </c>
     </row>
     <row r="120" spans="1:4" ht="30">
-      <c r="A120" s="27" t="s">
+      <c r="A120" s="21" t="s">
         <v>123</v>
       </c>
       <c r="B120" s="7" t="s">
@@ -19978,7 +20148,7 @@
       </c>
     </row>
     <row r="121" spans="1:4" ht="30">
-      <c r="A121" s="27" t="s">
+      <c r="A121" s="21" t="s">
         <v>124</v>
       </c>
       <c r="B121" s="7" t="s">
@@ -19993,7 +20163,7 @@
       </c>
     </row>
     <row r="122" spans="1:4" ht="30">
-      <c r="A122" s="27" t="s">
+      <c r="A122" s="21" t="s">
         <v>125</v>
       </c>
       <c r="B122" s="7" t="s">
@@ -20008,7 +20178,7 @@
       </c>
     </row>
     <row r="123" spans="1:4" ht="30">
-      <c r="A123" s="27" t="s">
+      <c r="A123" s="21" t="s">
         <v>126</v>
       </c>
       <c r="B123" s="7" t="s">
@@ -20023,7 +20193,7 @@
       </c>
     </row>
     <row r="124" spans="1:4" ht="30">
-      <c r="A124" s="27" t="s">
+      <c r="A124" s="21" t="s">
         <v>127</v>
       </c>
       <c r="B124" s="7" t="s">
@@ -20038,7 +20208,7 @@
       </c>
     </row>
     <row r="125" spans="1:4" ht="30">
-      <c r="A125" s="27" t="s">
+      <c r="A125" s="21" t="s">
         <v>128</v>
       </c>
       <c r="B125" s="7" t="s">
@@ -20053,7 +20223,7 @@
       </c>
     </row>
     <row r="126" spans="1:4" ht="30">
-      <c r="A126" s="27" t="s">
+      <c r="A126" s="21" t="s">
         <v>129</v>
       </c>
       <c r="B126" s="7" t="s">
@@ -20068,7 +20238,7 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="30">
-      <c r="A127" s="27" t="s">
+      <c r="A127" s="21" t="s">
         <v>130</v>
       </c>
       <c r="B127" s="7" t="s">
@@ -20083,7 +20253,7 @@
       </c>
     </row>
     <row r="128" spans="1:4" ht="30">
-      <c r="A128" s="27" t="s">
+      <c r="A128" s="21" t="s">
         <v>131</v>
       </c>
       <c r="B128" s="7" t="s">
@@ -20098,7 +20268,7 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="30">
-      <c r="A129" s="27" t="s">
+      <c r="A129" s="21" t="s">
         <v>132</v>
       </c>
       <c r="B129" s="7" t="s">
@@ -20113,7 +20283,7 @@
       </c>
     </row>
     <row r="130" spans="1:5" ht="30">
-      <c r="A130" s="27" t="s">
+      <c r="A130" s="21" t="s">
         <v>133</v>
       </c>
       <c r="B130" s="7" t="s">
@@ -20128,7 +20298,7 @@
       </c>
     </row>
     <row r="131" spans="1:5" ht="30">
-      <c r="A131" s="27" t="s">
+      <c r="A131" s="21" t="s">
         <v>134</v>
       </c>
       <c r="B131" s="7" t="s">
@@ -20143,7 +20313,7 @@
       </c>
     </row>
     <row r="132" spans="1:5" ht="30">
-      <c r="A132" s="27" t="s">
+      <c r="A132" s="21" t="s">
         <v>135</v>
       </c>
       <c r="B132" s="7" t="s">
@@ -20158,7 +20328,7 @@
       </c>
     </row>
     <row r="133" spans="1:5" ht="30">
-      <c r="A133" s="27" t="s">
+      <c r="A133" s="21" t="s">
         <v>136</v>
       </c>
       <c r="B133" s="7" t="s">
@@ -20173,7 +20343,7 @@
       </c>
     </row>
     <row r="134" spans="1:5" ht="30">
-      <c r="A134" s="27" t="s">
+      <c r="A134" s="21" t="s">
         <v>137</v>
       </c>
       <c r="B134" s="7" t="s">
@@ -20188,7 +20358,7 @@
       </c>
     </row>
     <row r="135" spans="1:5" ht="30">
-      <c r="A135" s="27" t="s">
+      <c r="A135" s="21" t="s">
         <v>138</v>
       </c>
       <c r="B135" s="7" t="s">
@@ -20203,7 +20373,7 @@
       </c>
     </row>
     <row r="136" spans="1:5" ht="30">
-      <c r="A136" s="27" t="s">
+      <c r="A136" s="21" t="s">
         <v>139</v>
       </c>
       <c r="B136" s="7" t="s">
@@ -20218,7 +20388,7 @@
       </c>
     </row>
     <row r="137" spans="1:5" ht="30">
-      <c r="A137" s="27" t="s">
+      <c r="A137" s="21" t="s">
         <v>140</v>
       </c>
       <c r="B137" s="7" t="s">
@@ -20233,7 +20403,7 @@
       </c>
     </row>
     <row r="138" spans="1:5" ht="30">
-      <c r="A138" s="27" t="s">
+      <c r="A138" s="21" t="s">
         <v>141</v>
       </c>
       <c r="B138" s="7" t="s">
@@ -20248,7 +20418,7 @@
       </c>
     </row>
     <row r="139" spans="1:5" ht="30">
-      <c r="A139" s="27" t="s">
+      <c r="A139" s="21" t="s">
         <v>142</v>
       </c>
       <c r="B139" s="7" t="s">
@@ -20263,7 +20433,7 @@
       </c>
     </row>
     <row r="140" spans="1:5" ht="30">
-      <c r="A140" s="27" t="s">
+      <c r="A140" s="21" t="s">
         <v>143</v>
       </c>
       <c r="B140" s="7" t="s">
@@ -20278,7 +20448,7 @@
       </c>
     </row>
     <row r="141" spans="1:5" ht="30">
-      <c r="A141" s="27" t="s">
+      <c r="A141" s="21" t="s">
         <v>144</v>
       </c>
       <c r="B141" s="7" t="s">
@@ -20293,7 +20463,7 @@
       </c>
     </row>
     <row r="142" spans="1:5" ht="30">
-      <c r="A142" s="27" t="s">
+      <c r="A142" s="21" t="s">
         <v>145</v>
       </c>
       <c r="B142" s="7" t="s">
@@ -20308,7 +20478,7 @@
       </c>
     </row>
     <row r="143" spans="1:5" ht="30">
-      <c r="A143" s="27" t="s">
+      <c r="A143" s="21" t="s">
         <v>146</v>
       </c>
       <c r="B143" s="7" t="s">
@@ -20323,34 +20493,34 @@
       </c>
     </row>
     <row r="144" spans="1:5" ht="20">
-      <c r="A144" s="13"/>
-      <c r="B144" s="13"/>
-      <c r="C144" s="16"/>
-      <c r="D144" s="13"/>
-      <c r="E144" s="13"/>
+      <c r="A144" s="55"/>
+      <c r="B144" s="55"/>
+      <c r="C144" s="58"/>
+      <c r="D144" s="55"/>
+      <c r="E144" s="57"/>
     </row>
     <row r="145" spans="1:5">
       <c r="C145" s="9"/>
     </row>
     <row r="146" spans="1:5" ht="20">
-      <c r="A146" s="14"/>
-      <c r="B146" s="15" t="s">
+      <c r="A146" s="59"/>
+      <c r="B146" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="C146" s="14"/>
-      <c r="D146" s="13"/>
-      <c r="E146" s="13" t="s">
+      <c r="C146" s="61"/>
+      <c r="D146" s="62"/>
+      <c r="E146" s="63" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="147" spans="1:5">
-      <c r="A147" s="14"/>
-      <c r="B147" s="12" t="s">
+      <c r="A147" s="59"/>
+      <c r="B147" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="C147" s="13"/>
-      <c r="D147" s="13"/>
-      <c r="E147" s="13"/>
+      <c r="C147" s="63"/>
+      <c r="D147" s="62"/>
+      <c r="E147" s="63"/>
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="6">
@@ -20488,11 +20658,11 @@
       </c>
     </row>
     <row r="157" spans="1:5" ht="20">
-      <c r="A157" s="13"/>
-      <c r="B157" s="13"/>
-      <c r="C157" s="16"/>
-      <c r="D157" s="13"/>
-      <c r="E157" s="13"/>
+      <c r="A157" s="62"/>
+      <c r="B157" s="62"/>
+      <c r="C157" s="64"/>
+      <c r="D157" s="62"/>
+      <c r="E157" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>